<commit_message>
add Bouri et al (2021)
</commit_message>
<xml_diff>
--- a/2021 Bouri et al  Int. Rev. Financial Anal/data.xlsx
+++ b/2021 Bouri et al  Int. Rev. Financial Anal/data.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="TRNR_6704edb52b374ea797c22bf9db85c2fe_471_7" hidden="1">#REF!</definedName>
-    <definedName name="TRNR_7ab5b74d6608410589f10ae4eeca94bb_2351_7" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="TRNR_1b392440abc04e9cb3e990595d2478b0_471_7" hidden="1">#REF!</definedName>
+    <definedName name="TRNR_a6a9d097d1b94ba486f951c38fb1e96f_2349_7" hidden="1">Sheet1!$A$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,6 +38,12 @@
     <t>Date</t>
   </si>
   <si>
+    <t>MSCI World</t>
+  </si>
+  <si>
+    <t>USD Index</t>
+  </si>
+  <si>
     <t>Gold</t>
   </si>
   <si>
@@ -45,12 +51,6 @@
   </si>
   <si>
     <t>Bond Index</t>
-  </si>
-  <si>
-    <t>USD Index</t>
-  </si>
-  <si>
-    <t>MSCI World</t>
   </si>
 </sst>
 </file>
@@ -395,10 +395,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F5139"/>
+  <dimension ref="A1:F5168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2314" workbookViewId="0">
+      <selection activeCell="C2342" sqref="C2342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,6 +407,7 @@
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -414,19 +415,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -46853,108 +46854,577 @@
       <c r="A2323" s="2">
         <v>43924</v>
       </c>
-      <c r="B2323">
-        <v>855.15</v>
-      </c>
-      <c r="C2323">
-        <v>211.71</v>
-      </c>
-      <c r="D2323">
+      <c r="B2323" s="3">
+        <v>859.33</v>
+      </c>
+      <c r="C2323" s="3">
+        <v>236.96</v>
+      </c>
+      <c r="D2323" s="3">
         <v>1776.8610000000001</v>
       </c>
-      <c r="E2323">
+      <c r="E2323" s="3">
         <v>100.58</v>
       </c>
-      <c r="F2323">
+      <c r="F2323" s="3">
         <v>103.7</v>
       </c>
     </row>
     <row r="2324" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2324" s="1"/>
+      <c r="A2324" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B2324" s="3">
+        <v>884.51</v>
+      </c>
+      <c r="C2324" s="3">
+        <v>218.07</v>
+      </c>
+      <c r="D2324" s="3">
+        <v>1881.4780000000001</v>
+      </c>
+      <c r="E2324" s="3">
+        <v>100.68</v>
+      </c>
+      <c r="F2324" s="3">
+        <v>105.69</v>
+      </c>
     </row>
     <row r="2325" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2325" s="1"/>
+      <c r="A2325" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B2325" s="3">
+        <v>879.18</v>
+      </c>
+      <c r="C2325" s="3">
+        <v>197.58</v>
+      </c>
+      <c r="D2325" s="3">
+        <v>1895.04</v>
+      </c>
+      <c r="E2325" s="3">
+        <v>99.9</v>
+      </c>
+      <c r="F2325" s="3">
+        <v>106.14</v>
+      </c>
     </row>
     <row r="2326" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2326" s="1"/>
+      <c r="A2326" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B2326" s="3">
+        <v>879.5</v>
+      </c>
+      <c r="C2326" s="3">
+        <v>209.32</v>
+      </c>
+      <c r="D2326" s="3">
+        <v>1940.0820000000001</v>
+      </c>
+      <c r="E2326" s="3">
+        <v>100.12</v>
+      </c>
+      <c r="F2326" s="3">
+        <v>107.07</v>
+      </c>
     </row>
     <row r="2327" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2327" s="1"/>
+      <c r="A2327" s="2">
+        <v>43930</v>
+      </c>
+      <c r="B2327" s="3">
+        <v>915.27</v>
+      </c>
+      <c r="C2327" s="3">
+        <v>194.37</v>
+      </c>
+      <c r="D2327" s="3">
+        <v>1970.671</v>
+      </c>
+      <c r="E2327" s="3">
+        <v>99.52</v>
+      </c>
+      <c r="F2327" s="3">
+        <v>109.94</v>
+      </c>
     </row>
     <row r="2328" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2328" s="1"/>
+      <c r="A2328" s="2">
+        <v>43931</v>
+      </c>
+      <c r="B2328" s="3">
+        <v>915.27</v>
+      </c>
+      <c r="C2328" s="3">
+        <v>194.37</v>
+      </c>
+      <c r="D2328" s="3">
+        <v>1971.9549999999999</v>
+      </c>
+      <c r="E2328" s="3">
+        <v>99.52</v>
+      </c>
+      <c r="F2328" s="3">
+        <v>109.94</v>
+      </c>
     </row>
     <row r="2329" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2329" s="1"/>
+      <c r="A2329" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B2329" s="3">
+        <v>919.78</v>
+      </c>
+      <c r="C2329" s="3">
+        <v>195.28</v>
+      </c>
+      <c r="D2329" s="3">
+        <v>1956.752</v>
+      </c>
+      <c r="E2329" s="3">
+        <v>99.35</v>
+      </c>
+      <c r="F2329" s="3">
+        <v>110.69</v>
+      </c>
     </row>
     <row r="2330" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2330" s="1"/>
+      <c r="A2330" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B2330" s="3">
+        <v>923.7</v>
+      </c>
+      <c r="C2330" s="3">
+        <v>181.64</v>
+      </c>
+      <c r="D2330" s="3">
+        <v>2006.8050000000001</v>
+      </c>
+      <c r="E2330" s="3">
+        <v>98.89</v>
+      </c>
+      <c r="F2330" s="3">
+        <v>109.88</v>
+      </c>
     </row>
     <row r="2331" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2331" s="1"/>
+      <c r="A2331" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B2331" s="3">
+        <v>908.72</v>
+      </c>
+      <c r="C2331" s="3">
+        <v>172.63</v>
+      </c>
+      <c r="D2331" s="3">
+        <v>1960.202</v>
+      </c>
+      <c r="E2331" s="3">
+        <v>99.46</v>
+      </c>
+      <c r="F2331" s="3">
+        <v>110.33</v>
+      </c>
     </row>
     <row r="2332" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2332" s="1"/>
+      <c r="A2332" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B2332" s="3">
+        <v>904.29</v>
+      </c>
+      <c r="C2332" s="3">
+        <v>169.25</v>
+      </c>
+      <c r="D2332" s="3">
+        <v>1964.326</v>
+      </c>
+      <c r="E2332" s="3">
+        <v>100.02</v>
+      </c>
+      <c r="F2332" s="3">
+        <v>110.54</v>
+      </c>
     </row>
     <row r="2333" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2333" s="1"/>
+      <c r="A2333" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B2333" s="3">
+        <v>887.12</v>
+      </c>
+      <c r="C2333" s="3">
+        <v>165.94</v>
+      </c>
+      <c r="D2333" s="3">
+        <v>2017.508</v>
+      </c>
+      <c r="E2333" s="3">
+        <v>99.78</v>
+      </c>
+      <c r="F2333" s="3">
+        <v>110.84</v>
+      </c>
     </row>
     <row r="2334" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2334" s="1"/>
+      <c r="A2334" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B2334" s="3">
+        <v>893.61</v>
+      </c>
+      <c r="C2334" s="3">
+        <v>135.44</v>
+      </c>
+      <c r="D2334" s="3">
+        <v>1994.027</v>
+      </c>
+      <c r="E2334" s="3">
+        <v>99.96</v>
+      </c>
+      <c r="F2334" s="3">
+        <v>110.1</v>
+      </c>
     </row>
     <row r="2335" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2335" s="1"/>
+      <c r="A2335" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B2335" s="3">
+        <v>881.4</v>
+      </c>
+      <c r="C2335" s="3">
+        <v>76.709999999999994</v>
+      </c>
+      <c r="D2335" s="3">
+        <v>1932.25</v>
+      </c>
+      <c r="E2335" s="3">
+        <v>100.26</v>
+      </c>
+      <c r="F2335" s="3">
+        <v>110.04</v>
+      </c>
     </row>
     <row r="2336" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2336" s="1"/>
-    </row>
-    <row r="2337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2337" s="1"/>
-    </row>
-    <row r="2338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2338" s="1"/>
-    </row>
-    <row r="2339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2339" s="1"/>
-    </row>
-    <row r="2340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2340" s="1"/>
-    </row>
-    <row r="2341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2341" s="1"/>
-    </row>
-    <row r="2342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2342" s="1"/>
-    </row>
-    <row r="2343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2343" s="1"/>
-    </row>
-    <row r="2344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2344" s="1"/>
-    </row>
-    <row r="2345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2345" s="1"/>
-    </row>
-    <row r="2346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2346" s="1"/>
-    </row>
-    <row r="2347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2347" s="1"/>
-    </row>
-    <row r="2348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2348" s="1"/>
-    </row>
-    <row r="2349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2349" s="1"/>
-    </row>
-    <row r="2350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2350" s="1"/>
-    </row>
-    <row r="2351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2351" s="1"/>
-    </row>
-    <row r="2352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2352" s="1"/>
+      <c r="A2336" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B2336" s="3">
+        <v>907.77</v>
+      </c>
+      <c r="C2336" s="3">
+        <v>91.36</v>
+      </c>
+      <c r="D2336" s="3">
+        <v>1968.268</v>
+      </c>
+      <c r="E2336" s="3">
+        <v>100.39</v>
+      </c>
+      <c r="F2336" s="3">
+        <v>109.87</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2337" s="2">
+        <v>43944</v>
+      </c>
+      <c r="B2337" s="3">
+        <v>911.48</v>
+      </c>
+      <c r="C2337" s="3">
+        <v>109.39</v>
+      </c>
+      <c r="D2337" s="3">
+        <v>1974.3820000000001</v>
+      </c>
+      <c r="E2337" s="3">
+        <v>100.43</v>
+      </c>
+      <c r="F2337" s="3">
+        <v>110.43</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2338" s="2">
+        <v>43945</v>
+      </c>
+      <c r="B2338" s="3">
+        <v>906.37</v>
+      </c>
+      <c r="C2338" s="3">
+        <v>112.31</v>
+      </c>
+      <c r="D2338" s="3">
+        <v>1987.6469999999999</v>
+      </c>
+      <c r="E2338" s="3">
+        <v>100.38</v>
+      </c>
+      <c r="F2338" s="3">
+        <v>110.48</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2339" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B2339" s="3">
+        <v>900.21</v>
+      </c>
+      <c r="C2339" s="3">
+        <v>84.73</v>
+      </c>
+      <c r="D2339" s="3">
+        <v>2022.4949999999999</v>
+      </c>
+      <c r="E2339" s="3">
+        <v>100.04</v>
+      </c>
+      <c r="F2339" s="3">
+        <v>110.07</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2340" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B2340" s="3">
+        <v>899.38</v>
+      </c>
+      <c r="C2340" s="3">
+        <v>81.81</v>
+      </c>
+      <c r="D2340" s="3">
+        <v>2023.3510000000001</v>
+      </c>
+      <c r="E2340" s="3">
+        <v>99.87</v>
+      </c>
+      <c r="F2340" s="3">
+        <v>110.01</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2341" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B2341" s="3">
+        <v>894.79</v>
+      </c>
+      <c r="C2341" s="3">
+        <v>88.88</v>
+      </c>
+      <c r="D2341" s="3">
+        <v>2070.7640000000001</v>
+      </c>
+      <c r="E2341" s="3">
+        <v>99.57</v>
+      </c>
+      <c r="F2341" s="3">
+        <v>110.57</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2342" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B2342" s="3">
+        <v>884.76</v>
+      </c>
+      <c r="C2342" s="3">
+        <v>101.57</v>
+      </c>
+      <c r="D2342" s="3">
+        <v>2052.8449999999998</v>
+      </c>
+      <c r="E2342" s="3">
+        <v>99.02</v>
+      </c>
+      <c r="F2342" s="3">
+        <v>110.1</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2343" s="2">
+        <v>43952</v>
+      </c>
+      <c r="B2343" s="3">
+        <v>888.27</v>
+      </c>
+      <c r="C2343" s="3">
+        <v>103.62</v>
+      </c>
+      <c r="D2343" s="3">
+        <v>2004.7850000000001</v>
+      </c>
+      <c r="E2343" s="3">
+        <v>99.08</v>
+      </c>
+      <c r="F2343" s="3">
+        <v>109.42</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2344" s="2">
+        <v>43955</v>
+      </c>
+      <c r="B2344" s="3">
+        <v>894.75</v>
+      </c>
+      <c r="C2344" s="3">
+        <v>105.89</v>
+      </c>
+      <c r="D2344" s="3">
+        <v>1997.7470000000001</v>
+      </c>
+      <c r="E2344" s="3">
+        <v>99.48</v>
+      </c>
+      <c r="F2344" s="3">
+        <v>109.62</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2345" s="2">
+        <v>43956</v>
+      </c>
+      <c r="B2345" s="3">
+        <v>893.34</v>
+      </c>
+      <c r="C2345" s="3">
+        <v>123.14</v>
+      </c>
+      <c r="D2345" s="3">
+        <v>2018.115</v>
+      </c>
+      <c r="E2345" s="3">
+        <v>99.71</v>
+      </c>
+      <c r="F2345" s="3">
+        <v>109.69</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2346" s="2">
+        <v>43957</v>
+      </c>
+      <c r="B2346" s="3">
+        <v>881.8</v>
+      </c>
+      <c r="C2346" s="3">
+        <v>119.1</v>
+      </c>
+      <c r="D2346" s="3">
+        <v>2007.597</v>
+      </c>
+      <c r="E2346" s="3">
+        <v>100.09</v>
+      </c>
+      <c r="F2346" s="3">
+        <v>108.67</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2347" s="2">
+        <v>43958</v>
+      </c>
+      <c r="B2347" s="3">
+        <v>901.29</v>
+      </c>
+      <c r="C2347" s="3">
+        <v>115.42</v>
+      </c>
+      <c r="D2347" s="3">
+        <v>2026.1220000000001</v>
+      </c>
+      <c r="E2347" s="3">
+        <v>99.89</v>
+      </c>
+      <c r="F2347" s="3">
+        <v>109.02</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2348" s="2">
+        <v>43959</v>
+      </c>
+      <c r="B2348" s="3">
+        <v>895.37</v>
+      </c>
+      <c r="C2348" s="3">
+        <v>121.77</v>
+      </c>
+      <c r="D2348" s="3">
+        <v>2061.886</v>
+      </c>
+      <c r="E2348" s="3">
+        <v>99.73</v>
+      </c>
+      <c r="F2348" s="3">
+        <v>108.65</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2349" s="2">
+        <v>43962</v>
+      </c>
+      <c r="B2349" s="3">
+        <v>887.23</v>
+      </c>
+      <c r="C2349" s="3">
+        <v>116.48</v>
+      </c>
+      <c r="D2349" s="3">
+        <v>2060.7020000000002</v>
+      </c>
+      <c r="E2349" s="3">
+        <v>100.24</v>
+      </c>
+      <c r="F2349" s="3">
+        <v>108.17</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2350" s="2">
+        <v>43963</v>
+      </c>
+      <c r="B2350" s="3">
+        <v>890.93</v>
+      </c>
+      <c r="C2350" s="3">
+        <v>120.51</v>
+      </c>
+      <c r="D2350" s="3">
+        <v>2034.058</v>
+      </c>
+      <c r="E2350" s="3">
+        <v>99.93</v>
+      </c>
+      <c r="F2350" s="3">
+        <v>108.64</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2351" s="3"/>
+      <c r="B2351" s="3"/>
+      <c r="C2351" s="3"/>
+      <c r="D2351" s="3"/>
+      <c r="E2351" s="3"/>
+      <c r="F2351" s="3"/>
+    </row>
+    <row r="2352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2352" s="3"/>
+      <c r="B2352" s="3"/>
+      <c r="C2352" s="3"/>
+      <c r="D2352" s="3"/>
+      <c r="E2352" s="3"/>
+      <c r="F2352" s="3"/>
     </row>
     <row r="2353" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2353" s="1"/>
@@ -55317,7 +55787,97 @@
     <row r="5139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5139" s="1"/>
     </row>
+    <row r="5140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5140" s="1"/>
+    </row>
+    <row r="5141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5141" s="1"/>
+    </row>
+    <row r="5142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5142" s="1"/>
+    </row>
+    <row r="5143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5143" s="1"/>
+    </row>
+    <row r="5144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5144" s="1"/>
+    </row>
+    <row r="5145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5145" s="1"/>
+    </row>
+    <row r="5146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5146" s="1"/>
+    </row>
+    <row r="5147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5147" s="1"/>
+    </row>
+    <row r="5148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5148" s="1"/>
+    </row>
+    <row r="5149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5149" s="1"/>
+    </row>
+    <row r="5150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5150" s="1"/>
+    </row>
+    <row r="5151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5151" s="1"/>
+    </row>
+    <row r="5152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5152" s="1"/>
+    </row>
+    <row r="5153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5153" s="1"/>
+    </row>
+    <row r="5154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5154" s="1"/>
+    </row>
+    <row r="5155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5155" s="1"/>
+    </row>
+    <row r="5156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5156" s="1"/>
+    </row>
+    <row r="5157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5157" s="1"/>
+    </row>
+    <row r="5158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5158" s="1"/>
+    </row>
+    <row r="5159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5159" s="1"/>
+    </row>
+    <row r="5160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5160" s="1"/>
+    </row>
+    <row r="5161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5161" s="1"/>
+    </row>
+    <row r="5162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5162" s="1"/>
+    </row>
+    <row r="5163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5163" s="1"/>
+    </row>
+    <row r="5164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5164" s="1"/>
+    </row>
+    <row r="5165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5165" s="1"/>
+    </row>
+    <row r="5166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5166" s="1"/>
+    </row>
+    <row r="5167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5167" s="1"/>
+    </row>
+    <row r="5168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5168" s="1"/>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="TRAFO" prompt="$A$1:$H$2350" sqref="A1"/>
+  </dataValidations>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.75"/>
   <pageSetup fitToHeight="0"/>
 </worksheet>

</xml_diff>